<commit_message>
sys dev report 2.0; awaiting internal feedback
</commit_message>
<xml_diff>
--- a/project/Report/sysdev/SysDev-ReportTasks.xlsx
+++ b/project/Report/sysdev/SysDev-ReportTasks.xlsx
@@ -94,18 +94,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -126,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -134,6 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -143,8 +138,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +421,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,99 +439,99 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="3">
         <v>1.2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="3">
         <v>1.3</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="3">
         <v>1.4</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="3">
         <v>2.1</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
@@ -550,16 +543,16 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -568,12 +561,12 @@
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="C10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -582,12 +575,12 @@
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="C11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -596,68 +589,68 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>